<commit_message>
all pages are checked
</commit_message>
<xml_diff>
--- a/car_data.xlsx
+++ b/car_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="252">
   <si>
     <t>Nom de la voiture</t>
   </si>
@@ -319,52 +319,457 @@
     <t>Alfa Romeo Giulietta</t>
   </si>
   <si>
-    <t>01.2018</t>
-  </si>
-  <si>
     <t>7cv</t>
   </si>
   <si>
     <t>1368cm³</t>
   </si>
   <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>Giulietta</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Classe C Kit AMG</t>
+  </si>
+  <si>
+    <t>15.02.2024</t>
+  </si>
+  <si>
+    <t>1600cm³</t>
+  </si>
+  <si>
+    <t>106 000 DT</t>
+  </si>
+  <si>
+    <t>Suzuki Dzire Glx</t>
+  </si>
+  <si>
+    <t>220 000km</t>
+  </si>
+  <si>
+    <t>12.02.2024</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Dzire</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz 220 KIT AMG</t>
+  </si>
+  <si>
+    <t>86 000km</t>
+  </si>
+  <si>
+    <t>9cv</t>
+  </si>
+  <si>
+    <t>2200cm³</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>95 000 DT</t>
+  </si>
+  <si>
+    <t>BMW Série 3 F30 PACK M</t>
+  </si>
+  <si>
+    <t>250 000km</t>
+  </si>
+  <si>
+    <t>10cv</t>
+  </si>
+  <si>
+    <t>10.02.2024</t>
+  </si>
+  <si>
+    <t>2000cm³</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Série 3</t>
+  </si>
+  <si>
+    <t>Fiat Fiorino</t>
+  </si>
+  <si>
+    <t>Utilitaire</t>
+  </si>
+  <si>
+    <t>09.02.2024</t>
+  </si>
+  <si>
+    <t>1400cm³</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Fiorino</t>
+  </si>
+  <si>
+    <t>36 000 DT</t>
+  </si>
+  <si>
+    <t>Citroën C4 Berline</t>
+  </si>
+  <si>
+    <t>210 000km</t>
+  </si>
+  <si>
+    <t>03.02.2024</t>
+  </si>
+  <si>
+    <t>1500cm³</t>
+  </si>
+  <si>
+    <t>Citroën</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>38 000 DT</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Classe E AMG</t>
+  </si>
+  <si>
+    <t>24 500km</t>
+  </si>
+  <si>
+    <t>Propulsion</t>
+  </si>
+  <si>
+    <t>02.02.2024</t>
+  </si>
+  <si>
+    <t>1700cm³</t>
+  </si>
+  <si>
+    <t>Classe E</t>
+  </si>
+  <si>
+    <t>Sous leasing                    295 400 DT</t>
+  </si>
+  <si>
+    <t>50 000km</t>
+  </si>
+  <si>
+    <t>1995cm³</t>
+  </si>
+  <si>
+    <t>Gris</t>
+  </si>
+  <si>
+    <t>150 000 DT</t>
+  </si>
+  <si>
+    <t>Ford Fiesta</t>
+  </si>
+  <si>
+    <t>293 000km</t>
+  </si>
+  <si>
+    <t>1242cm³</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Fiesta</t>
+  </si>
+  <si>
+    <t>30 000 DT</t>
+  </si>
+  <si>
+    <t>Land Rover Discovery SE</t>
+  </si>
+  <si>
+    <t>3 000km</t>
+  </si>
+  <si>
+    <t>16cv</t>
+  </si>
+  <si>
+    <t>Intégrale</t>
+  </si>
+  <si>
+    <t>2993cm³</t>
+  </si>
+  <si>
+    <t>Land Rover</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
+    <t>Non dédouané                    372 000 DT</t>
+  </si>
+  <si>
+    <t>Haval H6</t>
+  </si>
+  <si>
+    <t>66 000km</t>
+  </si>
+  <si>
+    <t>899cm³</t>
+  </si>
+  <si>
+    <t>Marron</t>
+  </si>
+  <si>
+    <t>Haval</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>85 000 DT</t>
+  </si>
+  <si>
+    <t>Chery Arrizo 3</t>
+  </si>
+  <si>
+    <t>44 000km</t>
+  </si>
+  <si>
+    <t>1497cm³</t>
+  </si>
+  <si>
+    <t>Chery</t>
+  </si>
+  <si>
+    <t>Arrizo 3</t>
+  </si>
+  <si>
+    <t>39 000 DT</t>
+  </si>
+  <si>
+    <t>Volkswagen Polo Sedan</t>
+  </si>
+  <si>
+    <t>124 000km</t>
+  </si>
+  <si>
+    <t>900cm³</t>
+  </si>
+  <si>
+    <t>Polo Sedan</t>
+  </si>
+  <si>
+    <t>40 000 DT</t>
+  </si>
+  <si>
+    <t>Skoda Octavia</t>
+  </si>
+  <si>
+    <t>Skoda</t>
+  </si>
+  <si>
+    <t>Octavia</t>
+  </si>
+  <si>
+    <t>70 000 DT</t>
+  </si>
+  <si>
+    <t>BAIC YX Kenbo S2</t>
+  </si>
+  <si>
+    <t>130 000km</t>
+  </si>
+  <si>
+    <t>1498cm³</t>
+  </si>
+  <si>
+    <t>BAIC YX</t>
+  </si>
+  <si>
+    <t>Kenbo S2</t>
+  </si>
+  <si>
+    <t>90 000km</t>
+  </si>
+  <si>
+    <t>12cv</t>
+  </si>
+  <si>
+    <t>Hyundai Coupe Sport</t>
+  </si>
+  <si>
+    <t>127 000km</t>
+  </si>
+  <si>
+    <t>Coupé</t>
+  </si>
+  <si>
+    <t>Coupe</t>
+  </si>
+  <si>
+    <t>Ford Ka</t>
+  </si>
+  <si>
+    <t>Compacte</t>
+  </si>
+  <si>
+    <t>01.02.2024</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>26 000 DT</t>
+  </si>
+  <si>
+    <t>Nissan Juke Toute option</t>
+  </si>
+  <si>
+    <t>Autres</t>
+  </si>
+  <si>
+    <t>1000cm³</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Juke</t>
+  </si>
+  <si>
+    <t>Volkswagen Golf 7</t>
+  </si>
+  <si>
+    <t>145 000km</t>
+  </si>
+  <si>
+    <t>04.03.2024</t>
+  </si>
+  <si>
+    <t>1599cm³</t>
+  </si>
+  <si>
+    <t>Golf 7</t>
+  </si>
+  <si>
+    <t>46 000 DT</t>
+  </si>
+  <si>
+    <t>Chery Tiggo 2</t>
+  </si>
+  <si>
+    <t>45 000km</t>
+  </si>
+  <si>
+    <t>26.02.2024</t>
+  </si>
+  <si>
+    <t>998cm³</t>
+  </si>
+  <si>
+    <t>Tiggo 2</t>
+  </si>
+  <si>
+    <t>Sous leasing                    49 400 DT</t>
+  </si>
+  <si>
+    <t>Peugeot 2008</t>
+  </si>
+  <si>
+    <t>175 000km</t>
+  </si>
+  <si>
+    <t>22.02.2024</t>
+  </si>
+  <si>
+    <t>1199cm³</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>03.2022</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>Alfa Romeo</t>
-  </si>
-  <si>
-    <t>Giulietta</t>
-  </si>
-  <si>
-    <t>01.2021</t>
+    <t>04.2019</t>
+  </si>
+  <si>
+    <t>11.2014</t>
+  </si>
+  <si>
+    <t>12.2018</t>
+  </si>
+  <si>
+    <t>03.2019</t>
+  </si>
+  <si>
+    <t>10.2020</t>
+  </si>
+  <si>
+    <t>09.2014</t>
+  </si>
+  <si>
+    <t>06.2016</t>
   </si>
   <si>
     <t>03.2020</t>
   </si>
   <si>
-    <t>10.2019</t>
-  </si>
-  <si>
-    <t>02.2019</t>
-  </si>
-  <si>
-    <t>05.2018</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>03.2019</t>
+    <t>11.2003</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>04.2015</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>11.2012</t>
+  </si>
+  <si>
+    <t>06.2013</t>
+  </si>
+  <si>
+    <t>05.2020</t>
+  </si>
+  <si>
+    <t>05.2016</t>
+  </si>
+  <si>
+    <t>07.2015</t>
+  </si>
+  <si>
+    <t>01.2019</t>
+  </si>
+  <si>
+    <t>04.2013</t>
+  </si>
+  <si>
+    <t>04.2014</t>
   </si>
   <si>
     <t>01.2020</t>
   </si>
   <si>
-    <t>12.2016</t>
+    <t>12.2015</t>
   </si>
 </sst>
 </file>
@@ -719,16 +1124,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L21" activeCellId="1" sqref="M22 L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="19" width="25.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
@@ -1435,8 +1837,8 @@
       <c r="C14" t="s">
         <v>83</v>
       </c>
-      <c r="D14" t="s">
-        <v>101</v>
+      <c r="D14">
+        <v>1.2018</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -1445,7 +1847,7 @@
         <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
         <v>25</v>
@@ -1457,7 +1859,7 @@
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L14" t="s">
         <v>40</v>
@@ -1468,17 +1870,17 @@
       <c r="N14" t="s">
         <v>41</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>103</v>
+      </c>
+      <c r="R14" t="s">
         <v>104</v>
-      </c>
-      <c r="P14" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>106</v>
-      </c>
-      <c r="R14" t="s">
-        <v>107</v>
       </c>
       <c r="S14" t="s">
         <v>57</v>
@@ -1486,25 +1888,25 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>108</v>
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>7.2015000000000002</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s">
         <v>25</v>
@@ -1513,48 +1915,48 @@
         <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="K15" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N15" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" t="s">
-        <v>104</v>
-      </c>
-      <c r="P15" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>4</v>
       </c>
       <c r="Q15" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="R15" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="S15" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="D16">
+        <v>1.2019</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
@@ -1569,72 +1971,72 @@
         <v>25</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J16" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="K16" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="L16" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="M16" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="N16" t="s">
         <v>41</v>
       </c>
-      <c r="O16" t="s">
-        <v>104</v>
-      </c>
-      <c r="P16" t="s">
-        <v>104</v>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
       </c>
       <c r="Q16" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="R16" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="S16" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>110</v>
+        <v>116</v>
+      </c>
+      <c r="D17">
+        <v>4.2012999999999998</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="L17" t="s">
         <v>40</v>
@@ -1643,98 +2045,98 @@
         <v>40</v>
       </c>
       <c r="N17" t="s">
-        <v>41</v>
-      </c>
-      <c r="O17" t="s">
-        <v>104</v>
-      </c>
-      <c r="P17" t="s">
-        <v>104</v>
+        <v>86</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>4</v>
       </c>
       <c r="Q17" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="R17" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="S17" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
+        <v>122</v>
+      </c>
+      <c r="D18">
+        <v>4.2013999999999996</v>
       </c>
       <c r="E18" t="s">
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="H18" t="s">
         <v>25</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="K18" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="L18" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="M18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N18" t="s">
-        <v>31</v>
-      </c>
-      <c r="O18" t="s">
-        <v>104</v>
-      </c>
-      <c r="P18" t="s">
-        <v>104</v>
+        <v>86</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
       </c>
       <c r="Q18" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="R18" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="S18" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>111</v>
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>1.202</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1746,110 +2148,110 @@
         <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="J19" t="s">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="K19" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="L19" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="M19" t="s">
         <v>40</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
-      </c>
-      <c r="O19" t="s">
-        <v>104</v>
-      </c>
-      <c r="P19" t="s">
-        <v>104</v>
+        <v>41</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
       </c>
       <c r="Q19" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="R19" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="S19" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>112</v>
+        <v>136</v>
+      </c>
+      <c r="D20">
+        <v>12.201499999999999</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="K20" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="M20" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="N20" t="s">
-        <v>113</v>
-      </c>
-      <c r="O20" t="s">
-        <v>113</v>
-      </c>
-      <c r="P20" t="s">
-        <v>113</v>
+        <v>41</v>
+      </c>
+      <c r="O20">
+        <v>5</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
       </c>
       <c r="Q20" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="R20" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="S20" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
+        <v>143</v>
+      </c>
+      <c r="D21">
+        <v>3.2021999999999999</v>
       </c>
       <c r="E21" t="s">
         <v>22</v>
@@ -1858,196 +2260,196 @@
         <v>71</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="H21" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="I21" t="s">
         <v>26</v>
       </c>
       <c r="J21" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="K21" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="L21" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="M21" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="N21" t="s">
-        <v>113</v>
-      </c>
-      <c r="O21" t="s">
-        <v>113</v>
-      </c>
-      <c r="P21" t="s">
-        <v>113</v>
+        <v>86</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
       </c>
       <c r="Q21" t="s">
         <v>73</v>
       </c>
       <c r="R21" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="S21" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>112</v>
+        <v>149</v>
+      </c>
+      <c r="D22">
+        <v>4.2019000000000002</v>
       </c>
       <c r="E22" t="s">
         <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J22" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="K22" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="N22" t="s">
-        <v>113</v>
-      </c>
-      <c r="O22" t="s">
-        <v>113</v>
-      </c>
-      <c r="P22" t="s">
-        <v>113</v>
+        <v>41</v>
+      </c>
+      <c r="O22">
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>4</v>
       </c>
       <c r="Q22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="R22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="S22" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
+        <v>154</v>
+      </c>
+      <c r="D23">
+        <v>11.2014</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="H23" t="s">
         <v>25</v>
       </c>
       <c r="I23" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="J23" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="K23" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="L23" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="M23" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="N23" t="s">
-        <v>86</v>
-      </c>
-      <c r="O23" t="s">
-        <v>113</v>
-      </c>
-      <c r="P23" t="s">
-        <v>113</v>
+        <v>41</v>
+      </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
       </c>
       <c r="Q23" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="R23" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="S23" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" t="s">
-        <v>116</v>
+        <v>160</v>
+      </c>
+      <c r="D24">
+        <v>12.2018</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
         <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
       <c r="I24" t="s">
         <v>84</v>
       </c>
       <c r="J24" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="K24" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="L24" t="s">
         <v>40</v>
@@ -2058,79 +2460,2026 @@
       <c r="N24" t="s">
         <v>86</v>
       </c>
-      <c r="O24" t="s">
-        <v>104</v>
-      </c>
-      <c r="P24" t="s">
-        <v>104</v>
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
       </c>
       <c r="Q24" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="R24" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="S24" t="s">
-        <v>91</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25">
+        <v>3.2019000000000002</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" t="s">
+        <v>169</v>
+      </c>
+      <c r="L25" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" t="s">
+        <v>170</v>
+      </c>
+      <c r="N25" t="s">
+        <v>86</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>171</v>
+      </c>
+      <c r="R25" t="s">
+        <v>172</v>
+      </c>
+      <c r="S25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26">
+        <v>10.202</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" t="s">
+        <v>176</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>4</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>177</v>
+      </c>
+      <c r="R26" t="s">
+        <v>178</v>
+      </c>
+      <c r="S26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27">
+        <v>9.2013999999999996</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>145</v>
+      </c>
+      <c r="K27" t="s">
+        <v>182</v>
+      </c>
+      <c r="L27" t="s">
+        <v>85</v>
+      </c>
+      <c r="M27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="P27">
+        <v>4</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>97</v>
+      </c>
+      <c r="R27" t="s">
+        <v>183</v>
+      </c>
+      <c r="S27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>6.2016</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>145</v>
+      </c>
+      <c r="K28" t="s">
+        <v>182</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O28">
+        <v>5</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>186</v>
+      </c>
+      <c r="R28" t="s">
+        <v>187</v>
+      </c>
+      <c r="S28" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29">
+        <v>12.2018</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
         <v>101</v>
       </c>
-      <c r="E25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" t="s">
+        <v>84</v>
+      </c>
+      <c r="J29" t="s">
+        <v>145</v>
+      </c>
+      <c r="K29" t="s">
+        <v>191</v>
+      </c>
+      <c r="L29" t="s">
+        <v>85</v>
+      </c>
+      <c r="M29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29">
+        <v>5</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>192</v>
+      </c>
+      <c r="R29" t="s">
+        <v>193</v>
+      </c>
+      <c r="S29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30">
+        <v>3.202</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>195</v>
+      </c>
+      <c r="H30" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30" t="s">
+        <v>145</v>
+      </c>
+      <c r="K30" t="s">
+        <v>125</v>
+      </c>
+      <c r="L30" t="s">
+        <v>170</v>
+      </c>
+      <c r="M30" t="s">
+        <v>170</v>
+      </c>
+      <c r="N30" t="s">
+        <v>86</v>
+      </c>
+      <c r="O30">
+        <v>5</v>
+      </c>
+      <c r="P30">
+        <v>5</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>171</v>
+      </c>
+      <c r="R30" t="s">
+        <v>172</v>
+      </c>
+      <c r="S30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31">
+        <v>11.2003</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
         <v>23</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>198</v>
+      </c>
+      <c r="J31" t="s">
+        <v>145</v>
+      </c>
+      <c r="K31" t="s">
+        <v>107</v>
+      </c>
+      <c r="L31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>79</v>
+      </c>
+      <c r="R31" t="s">
+        <v>199</v>
+      </c>
+      <c r="S31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32">
+        <v>4.2015000000000002</v>
+      </c>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>201</v>
+      </c>
+      <c r="J32" t="s">
+        <v>202</v>
+      </c>
+      <c r="K32" t="s">
+        <v>155</v>
+      </c>
+      <c r="L32" t="s">
+        <v>85</v>
+      </c>
+      <c r="M32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>156</v>
+      </c>
+      <c r="R32" t="s">
+        <v>203</v>
+      </c>
+      <c r="S32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33">
+        <v>11.2012</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" t="s">
+        <v>202</v>
+      </c>
+      <c r="K33" t="s">
+        <v>207</v>
+      </c>
+      <c r="L33" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" t="s">
+        <v>86</v>
+      </c>
+      <c r="O33">
+        <v>5</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>208</v>
+      </c>
+      <c r="R33" t="s">
+        <v>209</v>
+      </c>
+      <c r="S33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34">
+        <v>6.2012999999999998</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" t="s">
+        <v>212</v>
+      </c>
+      <c r="K34" t="s">
+        <v>213</v>
+      </c>
+      <c r="L34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" t="s">
+        <v>170</v>
+      </c>
+      <c r="N34" t="s">
+        <v>31</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+      <c r="P34">
+        <v>5</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>97</v>
+      </c>
+      <c r="R34" t="s">
+        <v>214</v>
+      </c>
+      <c r="S34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35">
+        <v>5.202</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
         <v>46</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H35" t="s">
         <v>25</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I35" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" t="s">
+        <v>218</v>
+      </c>
+      <c r="K35" t="s">
+        <v>219</v>
+      </c>
+      <c r="L35" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" t="s">
+        <v>40</v>
+      </c>
+      <c r="N35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O35">
+        <v>5</v>
+      </c>
+      <c r="P35">
+        <v>5</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>177</v>
+      </c>
+      <c r="R35" t="s">
+        <v>220</v>
+      </c>
+      <c r="S35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36">
+        <v>5.2016</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" t="s">
+        <v>84</v>
+      </c>
+      <c r="J36" t="s">
+        <v>224</v>
+      </c>
+      <c r="K36" t="s">
+        <v>225</v>
+      </c>
+      <c r="L36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36" t="s">
+        <v>41</v>
+      </c>
+      <c r="O36">
+        <v>5</v>
+      </c>
+      <c r="P36">
+        <v>5</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>48</v>
+      </c>
+      <c r="R36" t="s">
+        <v>226</v>
+      </c>
+      <c r="S36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" t="s">
+        <v>144</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>145</v>
+      </c>
+      <c r="K37" t="s">
+        <v>146</v>
+      </c>
+      <c r="L37" t="s">
+        <v>85</v>
+      </c>
+      <c r="M37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N37" t="s">
+        <v>86</v>
+      </c>
+      <c r="O37" t="s">
+        <v>228</v>
+      </c>
+      <c r="P37" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>73</v>
+      </c>
+      <c r="R37" t="s">
+        <v>147</v>
+      </c>
+      <c r="S37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>145</v>
+      </c>
+      <c r="K38" t="s">
+        <v>150</v>
+      </c>
+      <c r="L38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" t="s">
+        <v>151</v>
+      </c>
+      <c r="N38" t="s">
+        <v>41</v>
+      </c>
+      <c r="O38" t="s">
+        <v>228</v>
+      </c>
+      <c r="P38" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>73</v>
+      </c>
+      <c r="R38" t="s">
+        <v>74</v>
+      </c>
+      <c r="S38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" t="s">
+        <v>231</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" t="s">
         <v>37</v>
       </c>
-      <c r="J25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K25" t="s">
-        <v>38</v>
-      </c>
-      <c r="L25" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" t="s">
-        <v>40</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="J39" t="s">
+        <v>145</v>
+      </c>
+      <c r="K39" t="s">
+        <v>155</v>
+      </c>
+      <c r="L39" t="s">
+        <v>65</v>
+      </c>
+      <c r="M39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" t="s">
         <v>41</v>
       </c>
-      <c r="O25" t="s">
-        <v>104</v>
-      </c>
-      <c r="P25" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>55</v>
-      </c>
-      <c r="R25" t="s">
-        <v>93</v>
-      </c>
-      <c r="S25" t="s">
-        <v>94</v>
+      <c r="O39" t="s">
+        <v>228</v>
+      </c>
+      <c r="P39" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>156</v>
+      </c>
+      <c r="R39" t="s">
+        <v>157</v>
+      </c>
+      <c r="S39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>232</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" t="s">
+        <v>161</v>
+      </c>
+      <c r="H40" t="s">
+        <v>162</v>
+      </c>
+      <c r="I40" t="s">
+        <v>84</v>
+      </c>
+      <c r="J40" t="s">
+        <v>145</v>
+      </c>
+      <c r="K40" t="s">
+        <v>163</v>
+      </c>
+      <c r="L40" t="s">
+        <v>40</v>
+      </c>
+      <c r="M40" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" t="s">
+        <v>86</v>
+      </c>
+      <c r="O40" t="s">
+        <v>228</v>
+      </c>
+      <c r="P40" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>164</v>
+      </c>
+      <c r="R40" t="s">
+        <v>165</v>
+      </c>
+      <c r="S40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>233</v>
+      </c>
+      <c r="E41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" t="s">
+        <v>84</v>
+      </c>
+      <c r="J41" t="s">
+        <v>145</v>
+      </c>
+      <c r="K41" t="s">
+        <v>169</v>
+      </c>
+      <c r="L41" t="s">
+        <v>40</v>
+      </c>
+      <c r="M41" t="s">
+        <v>170</v>
+      </c>
+      <c r="N41" t="s">
+        <v>86</v>
+      </c>
+      <c r="O41" t="s">
+        <v>228</v>
+      </c>
+      <c r="P41" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>171</v>
+      </c>
+      <c r="R41" t="s">
+        <v>172</v>
+      </c>
+      <c r="S41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" t="s">
+        <v>145</v>
+      </c>
+      <c r="K42" t="s">
+        <v>176</v>
+      </c>
+      <c r="L42" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42" t="s">
+        <v>41</v>
+      </c>
+      <c r="O42" t="s">
+        <v>228</v>
+      </c>
+      <c r="P42" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>177</v>
+      </c>
+      <c r="R42" t="s">
+        <v>178</v>
+      </c>
+      <c r="S42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" t="s">
+        <v>145</v>
+      </c>
+      <c r="K43" t="s">
+        <v>182</v>
+      </c>
+      <c r="L43" t="s">
+        <v>85</v>
+      </c>
+      <c r="M43" t="s">
+        <v>40</v>
+      </c>
+      <c r="N43" t="s">
+        <v>41</v>
+      </c>
+      <c r="O43" t="s">
+        <v>228</v>
+      </c>
+      <c r="P43" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>97</v>
+      </c>
+      <c r="R43" t="s">
+        <v>183</v>
+      </c>
+      <c r="S43" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>236</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" t="s">
+        <v>71</v>
+      </c>
+      <c r="G44" t="s">
+        <v>72</v>
+      </c>
+      <c r="H44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" t="s">
+        <v>145</v>
+      </c>
+      <c r="K44" t="s">
+        <v>182</v>
+      </c>
+      <c r="L44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" t="s">
+        <v>40</v>
+      </c>
+      <c r="N44" t="s">
+        <v>86</v>
+      </c>
+      <c r="O44" t="s">
+        <v>228</v>
+      </c>
+      <c r="P44" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>186</v>
+      </c>
+      <c r="R44" t="s">
+        <v>187</v>
+      </c>
+      <c r="S44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" t="s">
+        <v>232</v>
+      </c>
+      <c r="E45" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" t="s">
+        <v>144</v>
+      </c>
+      <c r="I45" t="s">
+        <v>84</v>
+      </c>
+      <c r="J45" t="s">
+        <v>145</v>
+      </c>
+      <c r="K45" t="s">
+        <v>191</v>
+      </c>
+      <c r="L45" t="s">
+        <v>85</v>
+      </c>
+      <c r="M45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N45" t="s">
+        <v>31</v>
+      </c>
+      <c r="O45" t="s">
+        <v>228</v>
+      </c>
+      <c r="P45" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>192</v>
+      </c>
+      <c r="R45" t="s">
+        <v>193</v>
+      </c>
+      <c r="S45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" t="s">
+        <v>237</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>71</v>
+      </c>
+      <c r="G46" t="s">
+        <v>195</v>
+      </c>
+      <c r="H46" t="s">
+        <v>144</v>
+      </c>
+      <c r="I46" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" t="s">
+        <v>145</v>
+      </c>
+      <c r="K46" t="s">
+        <v>125</v>
+      </c>
+      <c r="L46" t="s">
+        <v>170</v>
+      </c>
+      <c r="M46" t="s">
+        <v>170</v>
+      </c>
+      <c r="N46" t="s">
+        <v>86</v>
+      </c>
+      <c r="O46" t="s">
+        <v>228</v>
+      </c>
+      <c r="P46" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>171</v>
+      </c>
+      <c r="R46" t="s">
+        <v>172</v>
+      </c>
+      <c r="S46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" t="s">
+        <v>198</v>
+      </c>
+      <c r="J47" t="s">
+        <v>145</v>
+      </c>
+      <c r="K47" t="s">
+        <v>107</v>
+      </c>
+      <c r="L47" t="s">
+        <v>78</v>
+      </c>
+      <c r="M47" t="s">
+        <v>40</v>
+      </c>
+      <c r="N47" t="s">
+        <v>41</v>
+      </c>
+      <c r="O47" t="s">
+        <v>228</v>
+      </c>
+      <c r="P47" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>79</v>
+      </c>
+      <c r="R47" t="s">
+        <v>199</v>
+      </c>
+      <c r="S47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" t="s">
+        <v>240</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" t="s">
+        <v>25</v>
+      </c>
+      <c r="I48" t="s">
+        <v>201</v>
+      </c>
+      <c r="J48" t="s">
+        <v>202</v>
+      </c>
+      <c r="K48" t="s">
+        <v>155</v>
+      </c>
+      <c r="L48" t="s">
+        <v>85</v>
+      </c>
+      <c r="M48" t="s">
+        <v>40</v>
+      </c>
+      <c r="N48" t="s">
+        <v>41</v>
+      </c>
+      <c r="O48" t="s">
+        <v>229</v>
+      </c>
+      <c r="P48" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>156</v>
+      </c>
+      <c r="R48" t="s">
+        <v>203</v>
+      </c>
+      <c r="S48" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" t="s">
+        <v>242</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" t="s">
+        <v>25</v>
+      </c>
+      <c r="I49" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49" t="s">
+        <v>202</v>
+      </c>
+      <c r="K49" t="s">
+        <v>207</v>
+      </c>
+      <c r="L49" t="s">
+        <v>40</v>
+      </c>
+      <c r="M49" t="s">
+        <v>40</v>
+      </c>
+      <c r="N49" t="s">
+        <v>86</v>
+      </c>
+      <c r="O49" t="s">
+        <v>228</v>
+      </c>
+      <c r="P49" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>208</v>
+      </c>
+      <c r="R49" t="s">
+        <v>209</v>
+      </c>
+      <c r="S49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
+      <c r="A50" t="s">
+        <v>210</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" t="s">
+        <v>243</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" t="s">
+        <v>212</v>
+      </c>
+      <c r="K50" t="s">
+        <v>213</v>
+      </c>
+      <c r="L50" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50" t="s">
+        <v>170</v>
+      </c>
+      <c r="N50" t="s">
+        <v>31</v>
+      </c>
+      <c r="O50" t="s">
+        <v>228</v>
+      </c>
+      <c r="P50" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>97</v>
+      </c>
+      <c r="R50" t="s">
+        <v>214</v>
+      </c>
+      <c r="S50" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
+      <c r="A51" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" t="s">
+        <v>244</v>
+      </c>
+      <c r="E51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" t="s">
+        <v>46</v>
+      </c>
+      <c r="H51" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" t="s">
+        <v>84</v>
+      </c>
+      <c r="J51" t="s">
+        <v>218</v>
+      </c>
+      <c r="K51" t="s">
+        <v>219</v>
+      </c>
+      <c r="L51" t="s">
+        <v>39</v>
+      </c>
+      <c r="M51" t="s">
+        <v>40</v>
+      </c>
+      <c r="N51" t="s">
+        <v>31</v>
+      </c>
+      <c r="O51" t="s">
+        <v>228</v>
+      </c>
+      <c r="P51" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>177</v>
+      </c>
+      <c r="R51" t="s">
+        <v>220</v>
+      </c>
+      <c r="S51" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" t="s">
+        <v>222</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" t="s">
+        <v>245</v>
+      </c>
+      <c r="E52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" t="s">
+        <v>84</v>
+      </c>
+      <c r="J52" t="s">
+        <v>224</v>
+      </c>
+      <c r="K52" t="s">
+        <v>225</v>
+      </c>
+      <c r="L52" t="s">
+        <v>30</v>
+      </c>
+      <c r="M52" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52" t="s">
+        <v>41</v>
+      </c>
+      <c r="O52" t="s">
+        <v>228</v>
+      </c>
+      <c r="P52" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>48</v>
+      </c>
+      <c r="R52" t="s">
+        <v>226</v>
+      </c>
+      <c r="S52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>246</v>
+      </c>
+      <c r="E53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" t="s">
+        <v>71</v>
+      </c>
+      <c r="G53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" t="s">
+        <v>26</v>
+      </c>
+      <c r="J53" t="s">
+        <v>106</v>
+      </c>
+      <c r="K53" t="s">
+        <v>107</v>
+      </c>
+      <c r="L53" t="s">
+        <v>40</v>
+      </c>
+      <c r="M53" t="s">
+        <v>40</v>
+      </c>
+      <c r="N53" t="s">
+        <v>86</v>
+      </c>
+      <c r="O53" t="s">
+        <v>228</v>
+      </c>
+      <c r="P53" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>73</v>
+      </c>
+      <c r="R53" t="s">
+        <v>74</v>
+      </c>
+      <c r="S53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" t="s">
+        <v>247</v>
+      </c>
+      <c r="E54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I54" t="s">
+        <v>26</v>
+      </c>
+      <c r="J54" t="s">
+        <v>111</v>
+      </c>
+      <c r="K54" t="s">
+        <v>47</v>
+      </c>
+      <c r="L54" t="s">
+        <v>112</v>
+      </c>
+      <c r="M54" t="s">
+        <v>112</v>
+      </c>
+      <c r="N54" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" t="s">
+        <v>228</v>
+      </c>
+      <c r="P54" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>113</v>
+      </c>
+      <c r="R54" t="s">
+        <v>114</v>
+      </c>
+      <c r="S54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="s">
+        <v>248</v>
+      </c>
+      <c r="E55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" t="s">
+        <v>25</v>
+      </c>
+      <c r="I55" t="s">
+        <v>26</v>
+      </c>
+      <c r="J55" t="s">
+        <v>111</v>
+      </c>
+      <c r="K55" t="s">
+        <v>118</v>
+      </c>
+      <c r="L55" t="s">
+        <v>40</v>
+      </c>
+      <c r="M55" t="s">
+        <v>40</v>
+      </c>
+      <c r="N55" t="s">
+        <v>86</v>
+      </c>
+      <c r="O55" t="s">
+        <v>228</v>
+      </c>
+      <c r="P55" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>73</v>
+      </c>
+      <c r="R55" t="s">
+        <v>119</v>
+      </c>
+      <c r="S55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
+        <v>249</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" t="s">
+        <v>26</v>
+      </c>
+      <c r="J56" t="s">
+        <v>124</v>
+      </c>
+      <c r="K56" t="s">
+        <v>125</v>
+      </c>
+      <c r="L56" t="s">
+        <v>85</v>
+      </c>
+      <c r="M56" t="s">
+        <v>40</v>
+      </c>
+      <c r="N56" t="s">
+        <v>86</v>
+      </c>
+      <c r="O56" t="s">
+        <v>229</v>
+      </c>
+      <c r="P56" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>126</v>
+      </c>
+      <c r="R56" t="s">
+        <v>127</v>
+      </c>
+      <c r="S56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" t="s">
+        <v>129</v>
+      </c>
+      <c r="J57" t="s">
+        <v>130</v>
+      </c>
+      <c r="K57" t="s">
+        <v>131</v>
+      </c>
+      <c r="L57" t="s">
+        <v>85</v>
+      </c>
+      <c r="M57" t="s">
+        <v>40</v>
+      </c>
+      <c r="N57" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" t="s">
+        <v>239</v>
+      </c>
+      <c r="P57" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>132</v>
+      </c>
+      <c r="R57" t="s">
+        <v>133</v>
+      </c>
+      <c r="S57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" t="s">
+        <v>46</v>
+      </c>
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
+      <c r="I58" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" t="s">
+        <v>137</v>
+      </c>
+      <c r="K58" t="s">
+        <v>138</v>
+      </c>
+      <c r="L58" t="s">
+        <v>30</v>
+      </c>
+      <c r="M58" t="s">
+        <v>40</v>
+      </c>
+      <c r="N58" t="s">
+        <v>41</v>
+      </c>
+      <c r="O58" t="s">
+        <v>228</v>
+      </c>
+      <c r="P58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>139</v>
+      </c>
+      <c r="R58" t="s">
+        <v>140</v>
+      </c>
+      <c r="S58" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>